<commit_message>
collect special veg data
</commit_message>
<xml_diff>
--- a/data summary.xlsx
+++ b/data summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\xfd_vegetable_price\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07CE434F-66A8-46C0-A11C-87C8BAF6E0EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E10720D-F5BA-4FCE-8106-A661AF131B33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="9375" xr2:uid="{C3A12845-B9DA-49FE-B2AD-3BE1D4E0D4F3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>水菜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,14 @@
   </si>
   <si>
     <t>每月节约</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>截至20180722的文件数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>footer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,47 +477,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD27477-08DA-453E-A49E-6A0841FE6703}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="2" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>